<commit_message>
More changes in Excel
</commit_message>
<xml_diff>
--- a/code_1/Setup.xlsx
+++ b/code_1/Setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,8 +106,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +149,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -300,7 +312,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -310,8 +322,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,50 +353,53 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -392,6 +408,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -724,7 +741,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -735,74 +752,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="12">
         <v>100</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12">
         <v>400</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12">
         <v>1000</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="1:14" ht="16" thickBot="1">
-      <c r="B4" s="15"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14">
       <c r="B5" s="3"/>
@@ -875,17 +892,17 @@
         <f>G6*H6/G3</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="10">
         <v>128</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="10">
         <v>0.16</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="11">
         <f>L6*SQRT(3)</f>
         <v>0.27712812921102037</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="11">
         <f>K6*L6/K3</f>
         <v>2.0480000000000002E-2</v>
       </c>
@@ -909,31 +926,31 @@
         <f>C7*D7/C3</f>
         <v>0.15</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="24">
         <v>128</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="24">
         <v>0.15</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="24">
         <f>H7*SQRT(3)</f>
         <v>0.25980762113533157</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="24">
         <f>G7*H7/G3</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="11">
         <v>128</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="11">
         <v>0.2</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="11">
         <f>L7*SQRT(3)</f>
         <v>0.34641016151377546</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="11">
         <f>K7*L7/K3</f>
         <v>2.5600000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
Minor changes in iterate.c
</commit_message>
<xml_diff>
--- a/code_1/Setup.xlsx
+++ b/code_1/Setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,15 +106,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,11 +142,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -312,7 +300,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,9 +310,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,11 +382,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="9">
     <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -408,7 +392,6 @@
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,7 +724,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -926,17 +909,17 @@
         <f>C7*D7/C3</f>
         <v>0.15</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="7">
         <v>128</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="7">
         <v>0.15</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="7">
         <f>H7*SQRT(3)</f>
         <v>0.25980762113533157</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="7">
         <f>G7*H7/G3</f>
         <v>4.8000000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
Cambio en el excel
</commit_message>
<xml_diff>
--- a/code_1/Setup.xlsx
+++ b/code_1/Setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>LID DRIVEN CAVITY</t>
   </si>
@@ -44,12 +44,15 @@
   <si>
     <t>Divergence</t>
   </si>
+  <si>
+    <t>Converge pero los resultados son malos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,8 +109,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +152,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -300,7 +315,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -310,15 +325,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,8 +395,17 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -392,6 +414,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,241 +744,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>100</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11">
         <v>400</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11">
         <v>1000</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="14"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" ht="16" thickBot="1">
-      <c r="B4" s="17"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="B5" s="3"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>30</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.08</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <f>D6*SQRT(3)</f>
         <v>0.13856406460551018</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f>C6*D6/C3</f>
         <v>2.4E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="23">
         <v>128</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="23">
         <v>0.1</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="24">
         <f>H6*SQRT(3)</f>
         <v>0.17320508075688773</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="24">
         <f>G6*H6/G3</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>128</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <v>0.16</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <f>L6*SQRT(3)</f>
         <v>0.27712812921102037</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <f>K6*L6/K3</f>
         <v>2.0480000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
         <v>30</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f>D7*SQRT(3)</f>
         <v>0.8660254037844386</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f>C7*D7/C3</f>
         <v>0.15</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>128</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.15</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f>H7*SQRT(3)</f>
         <v>0.25980762113533157</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <f>G7*H7/G3</f>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>128</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>0.2</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="10">
         <f>L7*SQRT(3)</f>
         <v>0.34641016151377546</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <f>K7*L7/K3</f>
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>75</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>0.16</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f>H8*SQRT(3)</f>
         <v>0.27712812921102037</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <f>G8*H8/G3</f>
         <v>0.03</v>
       </c>
     </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A12:E12"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="K3:N4"/>

</xml_diff>